<commit_message>
Updated preparation script for britannica dataset
</commit_message>
<xml_diff>
--- a/data-raw/emperors/britannica/britannica.xlsx
+++ b/data-raw/emperors/britannica/britannica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianialexandre/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-spo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{422FAE5F-D692-D04C-8207-0E2BE73E168F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D765F030-6E08-4D55-A209-7E42B4265C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="520" windowWidth="11800" windowHeight="14300" xr2:uid="{A606D1FD-5175-6D42-A4AE-DCA1F5FEA576}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A606D1FD-5175-6D42-A4AE-DCA1F5FEA576}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Birth</t>
-  </si>
-  <si>
-    <t>Death</t>
-  </si>
-  <si>
     <t>Augustus</t>
   </si>
   <si>
@@ -384,12 +378,18 @@
   <si>
     <t>April 22, 238</t>
   </si>
+  <si>
+    <t>reign_start</t>
+  </si>
+  <si>
+    <t>reign_end</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -751,36 +751,36 @@
   <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.399999999999999">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.399999999999999">
+      <c r="A3" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>14</v>
@@ -789,9 +789,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.399999999999999">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>37</v>
@@ -800,9 +800,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.399999999999999">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>41</v>
@@ -811,9 +811,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.399999999999999">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>54</v>
@@ -822,9 +822,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.399999999999999">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>68</v>
@@ -833,31 +833,31 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.399999999999999">
       <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.399999999999999">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.399999999999999">
+      <c r="A10" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>69</v>
@@ -866,9 +866,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.399999999999999">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>79</v>
@@ -877,9 +877,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17.399999999999999">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>81</v>
@@ -888,9 +888,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.399999999999999">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>96</v>
@@ -899,9 +899,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17.399999999999999">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>98</v>
@@ -910,9 +910,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17.399999999999999">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>117</v>
@@ -921,9 +921,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17.399999999999999">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>138</v>
@@ -932,9 +932,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17.399999999999999">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>161</v>
@@ -943,9 +943,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17.399999999999999">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>161</v>
@@ -954,9 +954,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17.399999999999999">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>177</v>
@@ -965,31 +965,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17.399999999999999">
       <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17.399999999999999">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.399999999999999">
+      <c r="A22" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>193</v>
@@ -998,9 +998,9 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="17.399999999999999">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>198</v>
@@ -1009,9 +1009,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17.399999999999999">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>209</v>
@@ -1020,9 +1020,9 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="17.399999999999999">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>217</v>
@@ -1031,9 +1031,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="17.399999999999999">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>218</v>
@@ -1042,9 +1042,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="17.399999999999999">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>222</v>
@@ -1053,9 +1053,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17.399999999999999">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>235</v>
@@ -1064,53 +1064,53 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="17.399999999999999">
       <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17.399999999999999">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.399999999999999">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.399999999999999">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.399999999999999">
+      <c r="A33" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="B33" s="1">
         <v>238</v>
@@ -1119,9 +1119,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="17.399999999999999">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>244</v>
@@ -1130,9 +1130,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="17.399999999999999">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>249</v>
@@ -1141,9 +1141,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="17.399999999999999">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>251</v>
@@ -1152,9 +1152,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="17.399999999999999">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>251</v>
@@ -1163,9 +1163,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="17.399999999999999">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>253</v>
@@ -1174,9 +1174,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="17.399999999999999">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>253</v>
@@ -1185,9 +1185,9 @@
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="17.399999999999999">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>253</v>
@@ -1196,9 +1196,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="17.399999999999999">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>268</v>
@@ -1207,9 +1207,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="17.399999999999999">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>270</v>
@@ -1218,9 +1218,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="17.399999999999999">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>270</v>
@@ -1229,9 +1229,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="17.399999999999999">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>275</v>
@@ -1240,20 +1240,20 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="17.399999999999999">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17.399999999999999">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>276</v>
@@ -1262,9 +1262,9 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="17.399999999999999">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>282</v>
@@ -1273,9 +1273,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="17.399999999999999">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>283</v>
@@ -1284,9 +1284,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="17.399999999999999">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>283</v>
@@ -1295,9 +1295,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="17.399999999999999">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>284</v>
@@ -1306,9 +1306,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="17.399999999999999">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>286</v>
@@ -1317,9 +1317,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="17.399999999999999">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>305</v>
@@ -1328,9 +1328,9 @@
         <v>306</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="17.399999999999999">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1">
         <v>305</v>
@@ -1339,9 +1339,9 @@
         <v>311</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="17.399999999999999">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>306</v>
@@ -1350,9 +1350,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="17.399999999999999">
       <c r="A55" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>306</v>
@@ -1361,9 +1361,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="17.399999999999999">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1">
         <v>306</v>
@@ -1372,9 +1372,9 @@
         <v>337</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="17.399999999999999">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1">
         <v>310</v>
@@ -1383,9 +1383,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="17.399999999999999">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>308</v>
@@ -1394,9 +1394,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="17.399999999999999">
       <c r="A59" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>337</v>
@@ -1405,9 +1405,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="17.399999999999999">
       <c r="A60" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>337</v>
@@ -1416,9 +1416,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="17.399999999999999">
       <c r="A61" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1">
         <v>337</v>
@@ -1427,9 +1427,9 @@
         <v>350</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="17.399999999999999">
       <c r="A62" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>351</v>
@@ -1438,9 +1438,9 @@
         <v>354</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="17.399999999999999">
       <c r="A63" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1">
         <v>361</v>
@@ -1449,9 +1449,9 @@
         <v>363</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="17.399999999999999">
       <c r="A64" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1">
         <v>363</v>
@@ -1460,9 +1460,9 @@
         <v>364</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="17.399999999999999">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1">
         <v>364</v>
@@ -1471,9 +1471,9 @@
         <v>375</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="17.399999999999999">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>364</v>
@@ -1482,9 +1482,9 @@
         <v>378</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="17.399999999999999">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1">
         <v>367</v>
@@ -1493,9 +1493,9 @@
         <v>383</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="17.399999999999999">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1">
         <v>375</v>
@@ -1504,9 +1504,9 @@
         <v>392</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="17.399999999999999">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1">
         <v>379</v>
@@ -1515,9 +1515,9 @@
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="17.399999999999999">
       <c r="A70" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1">
         <v>383</v>
@@ -1526,9 +1526,9 @@
         <v>395</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="17.399999999999999">
       <c r="A71" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1">
         <v>383</v>
@@ -1537,9 +1537,9 @@
         <v>388</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="17.399999999999999">
       <c r="A72" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1">
         <v>393</v>
@@ -1548,9 +1548,9 @@
         <v>395</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="17.399999999999999">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1">
         <v>408</v>
@@ -1559,9 +1559,9 @@
         <v>450</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="17.399999999999999">
       <c r="A74" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1">
         <v>421</v>
@@ -1570,9 +1570,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="17.399999999999999">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1">
         <v>425</v>
@@ -1581,9 +1581,9 @@
         <v>455</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="17.399999999999999">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1">
         <v>450</v>
@@ -1592,20 +1592,20 @@
         <v>457</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="17.399999999999999">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17.399999999999999">
       <c r="A78" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1">
         <v>455</v>
@@ -1614,9 +1614,9 @@
         <v>456</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="17.399999999999999">
       <c r="A79" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1">
         <v>457</v>
@@ -1625,9 +1625,9 @@
         <v>461</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="17.399999999999999">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1">
         <v>461</v>
@@ -1636,9 +1636,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="17.399999999999999">
       <c r="A81" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1">
         <v>467</v>
@@ -1647,20 +1647,20 @@
         <v>472</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="17.399999999999999">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17.399999999999999">
       <c r="A83" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1">
         <v>473</v>
@@ -1669,9 +1669,9 @@
         <v>474</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="17.399999999999999">
       <c r="A84" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1">
         <v>474</v>
@@ -1680,9 +1680,9 @@
         <v>475</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="17.399999999999999">
       <c r="A85" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1">
         <v>475</v>
@@ -1691,9 +1691,9 @@
         <v>476</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="17.399999999999999">
       <c r="A86" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1">
         <v>457</v>
@@ -1702,9 +1702,9 @@
         <v>474</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="17.399999999999999">
       <c r="A87" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1">
         <v>474</v>
@@ -1713,9 +1713,9 @@
         <v>474</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="17.399999999999999">
       <c r="A88" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B88" s="1">
         <v>474</v>

</xml_diff>